<commit_message>
adding new plant gathering code
</commit_message>
<xml_diff>
--- a/src/com/generic/config/DataSheet.xlsx
+++ b/src/com/generic/config/DataSheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\WS\RayCatch\src\com\generic\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tariq Abu Alrob\git\RayCatch\src\com\generic\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E325A34-8FB3-4E52-BA0C-775369FCECDB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81EF7816-056E-4EB3-9848-9A53B69DBFE0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29610" yWindow="-120" windowWidth="28110" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SetupBrowsers" sheetId="42" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="134">
   <si>
     <t>Browser</t>
   </si>
@@ -421,6 +421,12 @@
   </si>
   <si>
     <t>id</t>
+  </si>
+  <si>
+    <t>plants</t>
+  </si>
+  <si>
+    <t>Italy Milan,Italy Castera,Cyprus Nicosia,</t>
   </si>
 </sst>
 </file>
@@ -1117,7 +1123,7 @@
   </sheetPr>
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
@@ -1131,7 +1137,7 @@
     <col min="7" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="19" customFormat="1" ht="30">
+    <row r="1" spans="1:6" s="19" customFormat="1">
       <c r="A1" s="7" t="s">
         <v>20</v>
       </c>
@@ -1279,7 +1285,7 @@
   <dimension ref="A1:I51"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:I33"/>
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -2461,10 +2467,10 @@
   <sheetPr>
     <tabColor rgb="FF002060"/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -2473,10 +2479,11 @@
     <col min="2" max="2" width="10.140625" style="6" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="14.5703125" style="6" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="20.85546875" style="6" customWidth="1" collapsed="1"/>
-    <col min="5" max="16384" width="9.140625" style="6"/>
+    <col min="5" max="5" width="43.5703125" style="6" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" s="7" t="s">
         <v>131</v>
       </c>
@@ -2489,8 +2496,11 @@
       <c r="D1" s="7" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" s="7" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="4" t="s">
         <v>39</v>
       </c>
@@ -2502,6 +2512,9 @@
       </c>
       <c r="D2" s="30" t="s">
         <v>127</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>133</v>
       </c>
     </row>
   </sheetData>

</xml_diff>